<commit_message>
Rename application to Pedestrian Mid-block Crossing Application
</commit_message>
<xml_diff>
--- a/Metadata/Application_Tracking_Worksheet.xlsx
+++ b/Metadata/Application_Tracking_Worksheet.xlsx
@@ -27,7 +27,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Newton, Diane B.:</t>
         </r>
@@ -36,7 +36,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Leidos (OSADP Team) to fill in - this is the status of uploading the application to the OSADP.</t>
@@ -51,7 +51,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Newton, Diane B.:</t>
         </r>
@@ -60,7 +60,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 OSADP admin and uploader = any notes related to application/project status, OSADP upload status, etc.</t>
@@ -75,7 +75,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Newton, Diane B.:</t>
         </r>
@@ -84,7 +84,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Leidos (OSADP Team) to fill in based on upload package.</t>
@@ -99,7 +99,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Newton, Diane B.:</t>
         </r>
@@ -108,7 +108,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Leidos (OSADP Team) to fill in based on upload package.</t>
@@ -123,7 +123,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Newton, Diane B.:</t>
         </r>
@@ -132,7 +132,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Leidos (OSADP Team) to fill in based on upload package.</t>
@@ -147,7 +147,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Newton, Diane B.:</t>
         </r>
@@ -156,7 +156,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 uploader to complete; organization = company or agency, POC within that organization, Status = active, closed;  POP</t>
@@ -171,7 +171,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Newton, Diane B.:</t>
         </r>
@@ -180,7 +180,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Uploader to fill in: Name, Company/organization, telephone, email</t>
@@ -195,7 +195,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Newton, Diane B.:</t>
         </r>
@@ -204,7 +204,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 If known, uploader to provide who at USDOT is/has reviewed their application.</t>
@@ -219,7 +219,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Newton, Diane B.:</t>
         </r>
@@ -228,7 +228,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Uploader to check all that apply and add others if not listed. Status: draft or final. 508 = yes/no (for 508 conversion); USDOT = yes/no (USDOT format); link = if published, please provide link for access.</t>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>Contract Title:</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t>Smart Phone Based In-Vehicle Driver Warnings for Pedestrian Mid-Block Crossings</t>
+  </si>
+  <si>
+    <t>Pedestrian Mid-block Crossing Application</t>
   </si>
 </sst>
 </file>
@@ -438,14 +441,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -863,7 +866,7 @@
   <dimension ref="B1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C3:F5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -921,7 +924,9 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>

</xml_diff>